<commit_message>
finished: now represents actual state of parameter support on different platforms
</commit_message>
<xml_diff>
--- a/doc/misc/agent_parameters.xlsx
+++ b/doc/misc/agent_parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="334">
   <si>
     <t>Parameter</t>
   </si>
@@ -706,6 +706,318 @@
   </si>
   <si>
     <t>CPU load average for last 15 minutes</t>
+  </si>
+  <si>
+    <t>Net.RemoteShareStatus(*)</t>
+  </si>
+  <si>
+    <t>Net.RemoteShareStatusText(*)</t>
+  </si>
+  <si>
+    <t>Status of remote shared resource</t>
+  </si>
+  <si>
+    <t>Status of remote shared resource as text</t>
+  </si>
+  <si>
+    <t>System.AppAddressSpace</t>
+  </si>
+  <si>
+    <t>Address space available to applications (MB)</t>
+  </si>
+  <si>
+    <t>System.ServiceState(*)</t>
+  </si>
+  <si>
+    <t>State of system service</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.User</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.User(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.User</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.User(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.User</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.User(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (USER) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Nice</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Nice(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Nice</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Nice(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Nice</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Nice(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (NICE) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.System</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.System(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.System</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.System(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.System</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.System(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SYSTEM) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Idle</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Idle(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Idle</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Idle(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Idle</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Idle(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IDLE) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.IOWait</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.IOWait(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.IOWait</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.IOWait(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.IOWait</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.IOWait(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IOWAIT) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.IRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.IRQ(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.IRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.IRQ(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.IRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.IRQ(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (IRQ) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.SoftIRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.SoftIRQ(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.SoftIRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.SoftIRQ(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.SoftIRQ</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.SoftIRQ(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (SOFTIRQ) for last 15 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Steal</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage.Steal(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Steal</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage5.Steal(*)</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Steal</t>
+  </si>
+  <si>
+    <t>System.CPU.Usage15.Steal(*)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last minute (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last minute (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last 5 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last 5 minutes (percents, specific CPU)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last 15 minutes (percents, all CPUs)</t>
+  </si>
+  <si>
+    <t>Average CPU usage (STEAL) for last 15 minutes (percents, specific CPU)</t>
   </si>
 </sst>
 </file>
@@ -1058,11 +1370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:O162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
+      <pane ySplit="2" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L163" sqref="L163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2295,6 +2607,9 @@
       <c r="D29" t="s">
         <v>53</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>187</v>
       </c>
@@ -2302,6 +2617,18 @@
         <v>187</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N29" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O29" t="s">
@@ -2318,6 +2645,9 @@
       <c r="D30" t="s">
         <v>53</v>
       </c>
+      <c r="E30" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F30" s="3" t="s">
         <v>187</v>
       </c>
@@ -2325,6 +2655,18 @@
         <v>187</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N30" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2338,6 +2680,9 @@
       <c r="D31" t="s">
         <v>53</v>
       </c>
+      <c r="E31" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F31" s="3" t="s">
         <v>187</v>
       </c>
@@ -2345,6 +2690,18 @@
         <v>187</v>
       </c>
       <c r="I31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N31" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2358,6 +2715,9 @@
       <c r="D32" t="s">
         <v>53</v>
       </c>
+      <c r="E32" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F32" s="3" t="s">
         <v>187</v>
       </c>
@@ -2365,6 +2725,9 @@
         <v>187</v>
       </c>
       <c r="I32" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N32" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2378,6 +2741,9 @@
       <c r="D33" t="s">
         <v>53</v>
       </c>
+      <c r="E33" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F33" s="3" t="s">
         <v>187</v>
       </c>
@@ -2385,6 +2751,15 @@
         <v>187</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L33" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2398,6 +2773,9 @@
       <c r="D34" t="s">
         <v>53</v>
       </c>
+      <c r="E34" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I34" s="3" t="s">
         <v>187</v>
       </c>
@@ -2412,6 +2790,9 @@
       <c r="D35" t="s">
         <v>53</v>
       </c>
+      <c r="E35" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>187</v>
       </c>
@@ -2419,6 +2800,18 @@
         <v>187</v>
       </c>
       <c r="I35" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N35" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O35" t="s">
@@ -2435,6 +2828,9 @@
       <c r="D36" t="s">
         <v>53</v>
       </c>
+      <c r="E36" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F36" s="3" t="s">
         <v>187</v>
       </c>
@@ -2442,6 +2838,15 @@
         <v>187</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2455,6 +2860,9 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
+      <c r="E37" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F37" s="3" t="s">
         <v>187</v>
       </c>
@@ -2462,6 +2870,18 @@
         <v>187</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N37" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2475,6 +2895,9 @@
       <c r="D38" t="s">
         <v>53</v>
       </c>
+      <c r="E38" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F38" s="3" t="s">
         <v>187</v>
       </c>
@@ -2482,6 +2905,18 @@
         <v>187</v>
       </c>
       <c r="I38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N38" s="3" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2495,6 +2930,9 @@
       <c r="D39" t="s">
         <v>53</v>
       </c>
+      <c r="E39" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>187</v>
       </c>
@@ -2512,10 +2950,25 @@
       <c r="D40" t="s">
         <v>53</v>
       </c>
+      <c r="E40" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F40" s="3" t="s">
         <v>187</v>
       </c>
       <c r="I40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N40" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O40" t="s">
@@ -2538,6 +2991,18 @@
       <c r="I41" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="J41" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O41" t="s">
         <v>175</v>
       </c>
@@ -2558,102 +3023,111 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O43" t="s">
-        <v>162</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>231</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
         <v>53</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O44" t="s">
-        <v>163</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D45" t="s">
         <v>53</v>
       </c>
+      <c r="E45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G45" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O45" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
         <v>53</v>
       </c>
+      <c r="E46" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F46" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="N46" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="C47" t="s">
         <v>100</v>
@@ -2661,10 +3135,28 @@
       <c r="D47" t="s">
         <v>53</v>
       </c>
+      <c r="E47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O47" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
         <v>100</v>
@@ -2672,10 +3164,43 @@
       <c r="D48" t="s">
         <v>53</v>
       </c>
+      <c r="E48" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O48" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
         <v>100</v>
@@ -2683,10 +3208,13 @@
       <c r="D49" t="s">
         <v>53</v>
       </c>
+      <c r="E49" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
         <v>100</v>
@@ -2694,10 +3222,13 @@
       <c r="D50" t="s">
         <v>53</v>
       </c>
+      <c r="E50" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
         <v>100</v>
@@ -2705,10 +3236,13 @@
       <c r="D51" t="s">
         <v>53</v>
       </c>
+      <c r="E51" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
         <v>100</v>
@@ -2716,10 +3250,16 @@
       <c r="D52" t="s">
         <v>53</v>
       </c>
+      <c r="E52" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C53" t="s">
         <v>100</v>
@@ -2727,16 +3267,13 @@
       <c r="D53" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O53" t="s">
-        <v>166</v>
+      <c r="E53" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
         <v>100</v>
@@ -2744,16 +3281,16 @@
       <c r="D54" t="s">
         <v>53</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O54" t="s">
-        <v>167</v>
+      <c r="E54" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
       <c r="C55" t="s">
         <v>100</v>
@@ -2761,16 +3298,28 @@
       <c r="D55" t="s">
         <v>53</v>
       </c>
+      <c r="E55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G55" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O55" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
         <v>100</v>
@@ -2778,16 +3327,28 @@
       <c r="D56" t="s">
         <v>53</v>
       </c>
+      <c r="E56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G56" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
         <v>100</v>
@@ -2795,40 +3356,16 @@
       <c r="D57" t="s">
         <v>53</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="G57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="N57" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O57" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
         <v>100</v>
@@ -2836,16 +3373,28 @@
       <c r="D58" t="s">
         <v>53</v>
       </c>
+      <c r="F58" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G58" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H58" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
         <v>100</v>
@@ -2853,16 +3402,43 @@
       <c r="D59" t="s">
         <v>53</v>
       </c>
+      <c r="E59" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G59" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
         <v>100</v>
@@ -2870,224 +3446,377 @@
       <c r="D60" t="s">
         <v>53</v>
       </c>
+      <c r="E60" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G60" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H60" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O60" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="D61" t="s">
         <v>53</v>
       </c>
+      <c r="E61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O61" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
         <v>53</v>
       </c>
+      <c r="E62" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="M62" s="3" t="s">
+      <c r="J62" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O62" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="D63" t="s">
         <v>53</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O63" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D64" t="s">
         <v>53</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I64" s="3" t="s">
+      <c r="E64" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O64" t="s">
-        <v>228</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:15">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="C65" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D65" t="s">
         <v>53</v>
       </c>
+      <c r="E65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G65" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="H65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M65" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N65" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O65" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>52</v>
       </c>
       <c r="D66" t="s">
         <v>53</v>
       </c>
+      <c r="E66" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G66" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H66" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I66" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="M66" s="3" t="s">
+      <c r="J66" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L66" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N66" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O66" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:15">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>157</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
       </c>
       <c r="D67" t="s">
         <v>53</v>
       </c>
+      <c r="E67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G67" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="M67" s="3" t="s">
+      <c r="H67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N67" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O67" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:15">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>158</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
       </c>
       <c r="D68" t="s">
         <v>53</v>
       </c>
+      <c r="E68" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G68" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H68" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I68" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="M68" s="3" t="s">
+      <c r="J68" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N68" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O68" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:15">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>16</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
       </c>
       <c r="D69" t="s">
         <v>53</v>
       </c>
+      <c r="E69" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G69" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I69" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M69" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O69" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:15">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
       </c>
       <c r="D70" t="s">
         <v>53</v>
       </c>
+      <c r="E70" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G70" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I70" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="M70" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O70" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>52</v>
       </c>
       <c r="D71" t="s">
         <v>53</v>
       </c>
+      <c r="E71" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="G71" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I71" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M71" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O71" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:15">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D72" t="s">
         <v>53</v>
@@ -3101,41 +3830,26 @@
       <c r="G72" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="M72" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="N72" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O72" s="4" t="s">
-        <v>191</v>
+      <c r="O72" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:15">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D73" t="s">
         <v>53</v>
       </c>
+      <c r="E73" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F73" s="3" t="s">
         <v>187</v>
       </c>
@@ -3145,39 +3859,45 @@
       <c r="I73" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="M73" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O73" t="s">
-        <v>150</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:15">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="C74" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D74" t="s">
         <v>53</v>
       </c>
+      <c r="E74" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F74" s="3" t="s">
         <v>187</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="M74" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O74" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:15">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>274</v>
       </c>
       <c r="C75" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D75" t="s">
         <v>53</v>
@@ -3185,22 +3905,16 @@
       <c r="F75" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G75" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="O75" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:15">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>275</v>
       </c>
       <c r="C76" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D76" t="s">
         <v>53</v>
@@ -3208,19 +3922,13 @@
       <c r="F76" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="O76" t="s">
-        <v>149</v>
+        <v>281</v>
       </c>
     </row>
     <row r="77" spans="1:15">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>276</v>
       </c>
       <c r="C77" t="s">
         <v>52</v>
@@ -3228,28 +3936,16 @@
       <c r="D77" t="s">
         <v>53</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="F77" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M77" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="O77" t="s">
-        <v>108</v>
+        <v>282</v>
       </c>
     </row>
     <row r="78" spans="1:15">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>277</v>
       </c>
       <c r="C78" t="s">
         <v>52</v>
@@ -3260,19 +3956,13 @@
       <c r="F78" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G78" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="O78" t="s">
-        <v>119</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="1:15">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>278</v>
       </c>
       <c r="C79" t="s">
         <v>52</v>
@@ -3280,19 +3970,16 @@
       <c r="D79" t="s">
         <v>53</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="F79" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O79" t="s">
-        <v>109</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" spans="1:15">
       <c r="A80" t="s">
-        <v>120</v>
+        <v>279</v>
       </c>
       <c r="C80" t="s">
         <v>52</v>
@@ -3304,12 +3991,12 @@
         <v>187</v>
       </c>
       <c r="O80" t="s">
-        <v>121</v>
+        <v>285</v>
       </c>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>286</v>
       </c>
       <c r="C81" t="s">
         <v>52</v>
@@ -3317,22 +4004,22 @@
       <c r="D81" t="s">
         <v>53</v>
       </c>
+      <c r="E81" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F81" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>187</v>
+      <c r="M81" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O81" t="s">
-        <v>144</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:15">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>287</v>
       </c>
       <c r="C82" t="s">
         <v>52</v>
@@ -3340,22 +4027,22 @@
       <c r="D82" t="s">
         <v>53</v>
       </c>
+      <c r="E82" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F82" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>187</v>
+      <c r="M82" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O82" t="s">
-        <v>145</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:15">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>288</v>
       </c>
       <c r="C83" t="s">
         <v>52</v>
@@ -3363,16 +4050,22 @@
       <c r="D83" t="s">
         <v>53</v>
       </c>
-      <c r="I83" s="3" t="s">
-        <v>187</v>
+      <c r="E83" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M83" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O83" t="s">
-        <v>200</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:15">
       <c r="A84" t="s">
-        <v>199</v>
+        <v>289</v>
       </c>
       <c r="C84" t="s">
         <v>52</v>
@@ -3380,70 +4073,88 @@
       <c r="D84" t="s">
         <v>53</v>
       </c>
-      <c r="I84" s="3" t="s">
-        <v>187</v>
+      <c r="E84" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M84" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O84" t="s">
-        <v>201</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:15">
       <c r="A85" t="s">
-        <v>214</v>
+        <v>290</v>
       </c>
       <c r="C85" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D85" t="s">
         <v>53</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="E85" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>187</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O85" t="s">
-        <v>215</v>
+        <v>296</v>
       </c>
     </row>
     <row r="86" spans="1:15">
       <c r="A86" t="s">
-        <v>194</v>
+        <v>291</v>
       </c>
       <c r="C86" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D86" t="s">
         <v>53</v>
       </c>
-      <c r="I86" s="3" t="s">
-        <v>187</v>
+      <c r="E86" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M86" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O86" t="s">
-        <v>196</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87" spans="1:15">
       <c r="A87" t="s">
-        <v>195</v>
+        <v>298</v>
       </c>
       <c r="C87" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D87" t="s">
         <v>53</v>
       </c>
-      <c r="I87" s="3" t="s">
-        <v>187</v>
+      <c r="F87" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M87" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O87" t="s">
-        <v>197</v>
+        <v>304</v>
       </c>
     </row>
     <row r="88" spans="1:15">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>299</v>
       </c>
       <c r="C88" t="s">
         <v>52</v>
@@ -3454,19 +4165,16 @@
       <c r="F88" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G88" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>187</v>
+      <c r="M88" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O88" t="s">
-        <v>146</v>
+        <v>305</v>
       </c>
     </row>
     <row r="89" spans="1:15">
       <c r="A89" t="s">
-        <v>113</v>
+        <v>300</v>
       </c>
       <c r="C89" t="s">
         <v>52</v>
@@ -3477,152 +4185,122 @@
       <c r="F89" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>187</v>
+      <c r="M89" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O89" t="s">
-        <v>147</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" spans="1:15">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>301</v>
       </c>
       <c r="C90" t="s">
-        <v>193</v>
+        <v>52</v>
       </c>
       <c r="D90" t="s">
-        <v>107</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>188</v>
+        <v>53</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L90" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M90" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="N90" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="O90" s="4" t="s">
-        <v>192</v>
+      <c r="O90" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="91" spans="1:15">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D91" t="s">
         <v>53</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I91" s="3" t="s">
+      <c r="F91" s="3" t="s">
         <v>187</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O91" t="s">
-        <v>125</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:15">
       <c r="A92" t="s">
-        <v>122</v>
+        <v>303</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="D92" t="s">
         <v>53</v>
       </c>
-      <c r="G92" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I92" s="3" t="s">
-        <v>187</v>
+      <c r="F92" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O92" t="s">
-        <v>124</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:15">
       <c r="A93" t="s">
-        <v>21</v>
+        <v>250</v>
       </c>
       <c r="C93" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D93" t="s">
         <v>53</v>
       </c>
-      <c r="G93" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I93" s="3" t="s">
+      <c r="E93" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>187</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O93" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>251</v>
       </c>
       <c r="C94" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D94" t="s">
         <v>53</v>
       </c>
-      <c r="G94" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I94" s="3" t="s">
+      <c r="E94" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>187</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O94" t="s">
-        <v>139</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>252</v>
       </c>
       <c r="C95" t="s">
         <v>52</v>
@@ -3630,36 +4308,45 @@
       <c r="D95" t="s">
         <v>53</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>187</v>
+      <c r="E95" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O95" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:15">
       <c r="A96" t="s">
-        <v>23</v>
+        <v>253</v>
       </c>
       <c r="C96" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D96" t="s">
         <v>53</v>
       </c>
-      <c r="I96" s="3" t="s">
-        <v>187</v>
+      <c r="E96" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O96" t="s">
-        <v>138</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:15">
       <c r="A97" t="s">
-        <v>132</v>
+        <v>254</v>
       </c>
       <c r="C97" t="s">
         <v>52</v>
@@ -3667,50 +4354,68 @@
       <c r="D97" t="s">
         <v>53</v>
       </c>
-      <c r="I97" s="3" t="s">
-        <v>187</v>
+      <c r="E97" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M97" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O97" t="s">
-        <v>140</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>255</v>
       </c>
       <c r="C98" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D98" t="s">
         <v>53</v>
       </c>
-      <c r="I98" s="3" t="s">
-        <v>187</v>
+      <c r="E98" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M98" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O98" t="s">
-        <v>141</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" t="s">
-        <v>25</v>
+        <v>310</v>
       </c>
       <c r="C99" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D99" t="s">
         <v>53</v>
       </c>
-      <c r="I99" s="3" t="s">
-        <v>187</v>
+      <c r="E99" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M99" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O99" t="s">
-        <v>142</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" t="s">
-        <v>131</v>
+        <v>311</v>
       </c>
       <c r="C100" t="s">
         <v>52</v>
@@ -3718,33 +4423,45 @@
       <c r="D100" t="s">
         <v>53</v>
       </c>
-      <c r="I100" s="3" t="s">
-        <v>187</v>
+      <c r="E100" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M100" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O100" t="s">
-        <v>143</v>
+        <v>317</v>
       </c>
     </row>
     <row r="101" spans="1:15">
       <c r="A101" t="s">
-        <v>26</v>
+        <v>312</v>
       </c>
       <c r="C101" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D101" t="s">
         <v>53</v>
       </c>
-      <c r="I101" s="3" t="s">
-        <v>187</v>
+      <c r="E101" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M101" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O101" t="s">
-        <v>137</v>
+        <v>318</v>
       </c>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>313</v>
       </c>
       <c r="C102" t="s">
         <v>52</v>
@@ -3752,50 +4469,68 @@
       <c r="D102" t="s">
         <v>53</v>
       </c>
-      <c r="I102" s="3" t="s">
-        <v>187</v>
+      <c r="E102" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O102" t="s">
-        <v>134</v>
+        <v>319</v>
       </c>
     </row>
     <row r="103" spans="1:15">
       <c r="A103" t="s">
-        <v>27</v>
+        <v>314</v>
       </c>
       <c r="C103" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D103" t="s">
         <v>53</v>
       </c>
-      <c r="I103" s="3" t="s">
-        <v>187</v>
+      <c r="E103" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O103" t="s">
-        <v>135</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:15">
       <c r="A104" t="s">
-        <v>28</v>
+        <v>315</v>
       </c>
       <c r="C104" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D104" t="s">
         <v>53</v>
       </c>
-      <c r="I104" s="3" t="s">
-        <v>187</v>
+      <c r="E104" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M104" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O104" t="s">
-        <v>136</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:15">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>322</v>
       </c>
       <c r="C105" t="s">
         <v>52</v>
@@ -3803,128 +4538,1564 @@
       <c r="D105" t="s">
         <v>53</v>
       </c>
-      <c r="I105" s="3" t="s">
-        <v>187</v>
+      <c r="E105" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M105" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O105" t="s">
-        <v>133</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" t="s">
-        <v>29</v>
+        <v>323</v>
       </c>
       <c r="C106" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D106" t="s">
         <v>53</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L106" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="M106" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="N106" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O106" t="s">
-        <v>40</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:15">
       <c r="A107" t="s">
-        <v>30</v>
+        <v>324</v>
       </c>
       <c r="C107" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D107" t="s">
         <v>53</v>
       </c>
-      <c r="G107" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I107" s="3" t="s">
-        <v>187</v>
+      <c r="E107" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O107" t="s">
-        <v>39</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:15">
       <c r="A108" t="s">
-        <v>31</v>
+        <v>325</v>
       </c>
       <c r="C108" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D108" t="s">
         <v>53</v>
       </c>
+      <c r="E108" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M108" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="O108" t="s">
-        <v>38</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:15">
       <c r="A109" t="s">
-        <v>32</v>
+        <v>326</v>
       </c>
       <c r="C109" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D109" t="s">
         <v>53</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>187</v>
+      <c r="E109" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M109" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="O109" t="s">
-        <v>37</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" t="s">
+        <v>327</v>
+      </c>
+      <c r="C110" t="s">
+        <v>52</v>
+      </c>
+      <c r="D110" t="s">
+        <v>53</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M110" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O110" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
+      <c r="A111" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" t="s">
+        <v>52</v>
+      </c>
+      <c r="D111" t="s">
+        <v>53</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M111" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O111" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" t="s">
+        <v>263</v>
+      </c>
+      <c r="C112" t="s">
+        <v>52</v>
+      </c>
+      <c r="D112" t="s">
+        <v>53</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M112" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O112" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113" t="s">
+        <v>264</v>
+      </c>
+      <c r="C113" t="s">
+        <v>52</v>
+      </c>
+      <c r="D113" t="s">
+        <v>53</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O113" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114" t="s">
+        <v>265</v>
+      </c>
+      <c r="C114" t="s">
+        <v>52</v>
+      </c>
+      <c r="D114" t="s">
+        <v>53</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O114" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
+      <c r="A115" t="s">
+        <v>266</v>
+      </c>
+      <c r="C115" t="s">
+        <v>52</v>
+      </c>
+      <c r="D115" t="s">
+        <v>53</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M115" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O115" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116" t="s">
+        <v>267</v>
+      </c>
+      <c r="C116" t="s">
+        <v>52</v>
+      </c>
+      <c r="D116" t="s">
+        <v>53</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M116" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O116" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" t="s">
+        <v>52</v>
+      </c>
+      <c r="D117" t="s">
+        <v>53</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O117" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="A118" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" t="s">
+        <v>52</v>
+      </c>
+      <c r="D118" t="s">
+        <v>53</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O118" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="A119" t="s">
+        <v>240</v>
+      </c>
+      <c r="C119" t="s">
+        <v>52</v>
+      </c>
+      <c r="D119" t="s">
+        <v>53</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O119" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" t="s">
+        <v>52</v>
+      </c>
+      <c r="D120" t="s">
+        <v>53</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O120" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" t="s">
+        <v>52</v>
+      </c>
+      <c r="D121" t="s">
+        <v>53</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O121" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" t="s">
+        <v>243</v>
+      </c>
+      <c r="C122" t="s">
+        <v>52</v>
+      </c>
+      <c r="D122" t="s">
+        <v>53</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O122" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15">
+      <c r="A123" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" t="s">
+        <v>36</v>
+      </c>
+      <c r="D123" t="s">
+        <v>53</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O123" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15">
+      <c r="A124" t="s">
+        <v>114</v>
+      </c>
+      <c r="C124" t="s">
+        <v>54</v>
+      </c>
+      <c r="D124" t="s">
+        <v>53</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="A125" t="s">
+        <v>115</v>
+      </c>
+      <c r="C125" t="s">
+        <v>54</v>
+      </c>
+      <c r="D125" t="s">
+        <v>53</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" t="s">
+        <v>116</v>
+      </c>
+      <c r="C126" t="s">
+        <v>54</v>
+      </c>
+      <c r="D126" t="s">
+        <v>53</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O126" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" t="s">
+        <v>117</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+      <c r="D127" t="s">
+        <v>53</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O127" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" t="s">
+        <v>105</v>
+      </c>
+      <c r="C128" t="s">
+        <v>52</v>
+      </c>
+      <c r="D128" t="s">
+        <v>53</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O128" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15">
+      <c r="A129" t="s">
+        <v>118</v>
+      </c>
+      <c r="C129" t="s">
+        <v>52</v>
+      </c>
+      <c r="D129" t="s">
+        <v>53</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O129" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
+      <c r="A130" t="s">
+        <v>106</v>
+      </c>
+      <c r="C130" t="s">
+        <v>52</v>
+      </c>
+      <c r="D130" t="s">
+        <v>53</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O130" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
+      <c r="A131" t="s">
+        <v>120</v>
+      </c>
+      <c r="C131" t="s">
+        <v>52</v>
+      </c>
+      <c r="D131" t="s">
+        <v>53</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O131" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
+      <c r="A132" t="s">
+        <v>110</v>
+      </c>
+      <c r="C132" t="s">
+        <v>52</v>
+      </c>
+      <c r="D132" t="s">
+        <v>53</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O132" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15">
+      <c r="A133" t="s">
+        <v>111</v>
+      </c>
+      <c r="C133" t="s">
+        <v>52</v>
+      </c>
+      <c r="D133" t="s">
+        <v>53</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O133" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15">
+      <c r="A134" t="s">
+        <v>198</v>
+      </c>
+      <c r="C134" t="s">
+        <v>52</v>
+      </c>
+      <c r="D134" t="s">
+        <v>53</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O134" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15">
+      <c r="A135" t="s">
+        <v>199</v>
+      </c>
+      <c r="C135" t="s">
+        <v>52</v>
+      </c>
+      <c r="D135" t="s">
+        <v>53</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O135" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15">
+      <c r="A136" t="s">
+        <v>214</v>
+      </c>
+      <c r="C136" t="s">
+        <v>35</v>
+      </c>
+      <c r="D136" t="s">
+        <v>53</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M136" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O136" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15">
+      <c r="A137" t="s">
+        <v>194</v>
+      </c>
+      <c r="C137" t="s">
+        <v>101</v>
+      </c>
+      <c r="D137" t="s">
+        <v>53</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O137" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15">
+      <c r="A138" t="s">
+        <v>195</v>
+      </c>
+      <c r="C138" t="s">
+        <v>101</v>
+      </c>
+      <c r="D138" t="s">
+        <v>53</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O138" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15">
+      <c r="A139" t="s">
+        <v>112</v>
+      </c>
+      <c r="C139" t="s">
+        <v>52</v>
+      </c>
+      <c r="D139" t="s">
+        <v>53</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O139" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15">
+      <c r="A140" t="s">
+        <v>113</v>
+      </c>
+      <c r="C140" t="s">
+        <v>52</v>
+      </c>
+      <c r="D140" t="s">
+        <v>53</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O140" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15">
+      <c r="A141" t="s">
+        <v>92</v>
+      </c>
+      <c r="C141" t="s">
+        <v>193</v>
+      </c>
+      <c r="D141" t="s">
+        <v>107</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O141" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15">
+      <c r="A142" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" t="s">
+        <v>100</v>
+      </c>
+      <c r="D142" t="s">
+        <v>53</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N142" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O142" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15">
+      <c r="A143" t="s">
+        <v>122</v>
+      </c>
+      <c r="C143" t="s">
+        <v>123</v>
+      </c>
+      <c r="D143" t="s">
+        <v>53</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N143" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O143" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15">
+      <c r="A144" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144" t="s">
+        <v>100</v>
+      </c>
+      <c r="D144" t="s">
+        <v>53</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O144" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
+      <c r="A145" t="s">
+        <v>22</v>
+      </c>
+      <c r="C145" t="s">
+        <v>100</v>
+      </c>
+      <c r="D145" t="s">
+        <v>53</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N145" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O145" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15">
+      <c r="A146" t="s">
+        <v>128</v>
+      </c>
+      <c r="C146" t="s">
+        <v>52</v>
+      </c>
+      <c r="D146" t="s">
+        <v>53</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N146" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O146" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15">
+      <c r="A147" t="s">
+        <v>23</v>
+      </c>
+      <c r="C147" t="s">
+        <v>100</v>
+      </c>
+      <c r="D147" t="s">
+        <v>53</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N147" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O147" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
+      <c r="A148" t="s">
+        <v>132</v>
+      </c>
+      <c r="C148" t="s">
+        <v>52</v>
+      </c>
+      <c r="D148" t="s">
+        <v>53</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O148" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15">
+      <c r="A149" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" t="s">
+        <v>100</v>
+      </c>
+      <c r="D149" t="s">
+        <v>53</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N149" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O149" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15">
+      <c r="A150" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" t="s">
+        <v>100</v>
+      </c>
+      <c r="D150" t="s">
+        <v>53</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N150" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O150" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15">
+      <c r="A151" t="s">
+        <v>131</v>
+      </c>
+      <c r="C151" t="s">
+        <v>52</v>
+      </c>
+      <c r="D151" t="s">
+        <v>53</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N151" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O151" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15">
+      <c r="A152" t="s">
+        <v>26</v>
+      </c>
+      <c r="C152" t="s">
+        <v>100</v>
+      </c>
+      <c r="D152" t="s">
+        <v>53</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N152" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O152" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15">
+      <c r="A153" t="s">
+        <v>129</v>
+      </c>
+      <c r="C153" t="s">
+        <v>52</v>
+      </c>
+      <c r="D153" t="s">
+        <v>53</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O153" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15">
+      <c r="A154" t="s">
+        <v>27</v>
+      </c>
+      <c r="C154" t="s">
+        <v>100</v>
+      </c>
+      <c r="D154" t="s">
+        <v>53</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O154" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15">
+      <c r="A155" t="s">
+        <v>28</v>
+      </c>
+      <c r="C155" t="s">
+        <v>100</v>
+      </c>
+      <c r="D155" t="s">
+        <v>53</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N155" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O155" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15">
+      <c r="A156" t="s">
+        <v>130</v>
+      </c>
+      <c r="C156" t="s">
+        <v>52</v>
+      </c>
+      <c r="D156" t="s">
+        <v>53</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N156" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O156" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
+      <c r="A157" t="s">
+        <v>29</v>
+      </c>
+      <c r="C157" t="s">
+        <v>36</v>
+      </c>
+      <c r="D157" t="s">
+        <v>53</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O157" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15">
+      <c r="A158" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" t="s">
+        <v>101</v>
+      </c>
+      <c r="D158" t="s">
+        <v>53</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O158" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15">
+      <c r="A159" t="s">
+        <v>236</v>
+      </c>
+      <c r="C159" t="s">
+        <v>35</v>
+      </c>
+      <c r="D159" t="s">
+        <v>53</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N159" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O159" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15">
+      <c r="A160" t="s">
+        <v>31</v>
+      </c>
+      <c r="C160" t="s">
+        <v>101</v>
+      </c>
+      <c r="D160" t="s">
+        <v>53</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H160" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J160" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K160" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O160" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15">
+      <c r="A161" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" t="s">
+        <v>36</v>
+      </c>
+      <c r="D161" t="s">
+        <v>53</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N161" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O161" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15">
+      <c r="A162" t="s">
         <v>33</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C162" t="s">
         <v>35</v>
       </c>
-      <c r="D110" t="s">
-        <v>53</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O110" t="s">
+      <c r="D162" t="s">
+        <v>53</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O162" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated agent param matrix
</commit_message>
<xml_diff>
--- a/doc/misc/agent_parameters.xlsx
+++ b/doc/misc/agent_parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="342">
   <si>
     <t>Parameter</t>
   </si>
@@ -1030,6 +1030,18 @@
   </si>
   <si>
     <t>Percentage of available physical memory</t>
+  </si>
+  <si>
+    <t>System.Memory.Virtual.Active</t>
+  </si>
+  <si>
+    <t>System.Memory.Virtual.ActivePerc</t>
+  </si>
+  <si>
+    <t>Active virtual memory</t>
+  </si>
+  <si>
+    <t>Percentage of active virtual memory</t>
   </si>
 </sst>
 </file>
@@ -1382,11 +1394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O164"/>
+  <dimension ref="A1:O166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3156,6 +3168,12 @@
       <c r="G47" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J47" s="3" t="s">
         <v>187</v>
       </c>
@@ -3268,6 +3286,9 @@
       <c r="H52" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I52" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
@@ -3299,6 +3320,9 @@
       <c r="H54" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I54" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
@@ -3322,6 +3346,9 @@
       <c r="H55" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I55" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="K55" s="3" t="s">
         <v>187</v>
       </c>
@@ -3351,6 +3378,9 @@
       <c r="H56" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I56" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="K56" s="3" t="s">
         <v>187</v>
       </c>
@@ -3394,6 +3424,9 @@
       <c r="H58" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I58" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J58" s="3" t="s">
         <v>187</v>
       </c>
@@ -3470,6 +3503,9 @@
       <c r="H60" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I60" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="K60" s="3" t="s">
         <v>187</v>
       </c>
@@ -3499,6 +3535,9 @@
       <c r="H61" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I61" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J61" s="3" t="s">
         <v>187</v>
       </c>
@@ -3528,6 +3567,9 @@
       <c r="G62" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I62" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J62" s="3" t="s">
         <v>187</v>
       </c>
@@ -3758,6 +3800,9 @@
       <c r="G69" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H69" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I69" s="3" t="s">
         <v>187</v>
       </c>
@@ -3787,6 +3832,9 @@
       <c r="G70" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H70" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M70" s="3" t="s">
         <v>187</v>
       </c>
@@ -3813,6 +3861,9 @@
       <c r="G71" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H71" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I71" s="3" t="s">
         <v>187</v>
       </c>
@@ -3842,6 +3893,9 @@
       <c r="G72" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H72" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M72" s="3" t="s">
         <v>187</v>
       </c>
@@ -3868,6 +3922,9 @@
       <c r="G73" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H73" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I73" s="3" t="s">
         <v>187</v>
       </c>
@@ -3897,6 +3954,9 @@
       <c r="G74" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H74" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M74" s="3" t="s">
         <v>187</v>
       </c>
@@ -3917,6 +3977,9 @@
       <c r="F75" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H75" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O75" t="s">
         <v>280</v>
       </c>
@@ -3934,6 +3997,9 @@
       <c r="F76" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H76" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O76" t="s">
         <v>281</v>
       </c>
@@ -3951,6 +4017,9 @@
       <c r="F77" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H77" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O77" t="s">
         <v>282</v>
       </c>
@@ -3968,6 +4037,9 @@
       <c r="F78" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H78" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O78" t="s">
         <v>283</v>
       </c>
@@ -3985,6 +4057,9 @@
       <c r="F79" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H79" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O79" t="s">
         <v>284</v>
       </c>
@@ -4002,6 +4077,9 @@
       <c r="F80" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H80" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O80" t="s">
         <v>285</v>
       </c>
@@ -4022,6 +4100,9 @@
       <c r="F81" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H81" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M81" s="3" t="s">
         <v>188</v>
       </c>
@@ -4045,6 +4126,9 @@
       <c r="F82" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H82" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M82" s="3" t="s">
         <v>188</v>
       </c>
@@ -4068,6 +4152,9 @@
       <c r="F83" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H83" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M83" s="3" t="s">
         <v>188</v>
       </c>
@@ -4091,6 +4178,9 @@
       <c r="F84" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H84" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M84" s="3" t="s">
         <v>188</v>
       </c>
@@ -4114,6 +4204,9 @@
       <c r="F85" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H85" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M85" s="3" t="s">
         <v>188</v>
       </c>
@@ -4137,6 +4230,9 @@
       <c r="F86" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H86" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M86" s="3" t="s">
         <v>188</v>
       </c>
@@ -4157,6 +4253,9 @@
       <c r="F87" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H87" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M87" s="3" t="s">
         <v>188</v>
       </c>
@@ -4177,6 +4276,9 @@
       <c r="F88" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H88" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M88" s="3" t="s">
         <v>188</v>
       </c>
@@ -4197,6 +4299,9 @@
       <c r="F89" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H89" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M89" s="3" t="s">
         <v>188</v>
       </c>
@@ -4217,6 +4322,9 @@
       <c r="F90" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H90" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M90" s="3" t="s">
         <v>188</v>
       </c>
@@ -4237,6 +4345,9 @@
       <c r="F91" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H91" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M91" s="3" t="s">
         <v>188</v>
       </c>
@@ -4257,6 +4368,9 @@
       <c r="F92" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H92" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M92" s="3" t="s">
         <v>188</v>
       </c>
@@ -4280,6 +4394,9 @@
       <c r="F93" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H93" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M93" s="3" t="s">
         <v>188</v>
       </c>
@@ -4303,6 +4420,9 @@
       <c r="F94" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H94" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M94" s="3" t="s">
         <v>188</v>
       </c>
@@ -4326,6 +4446,9 @@
       <c r="F95" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H95" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M95" s="3" t="s">
         <v>188</v>
       </c>
@@ -4349,6 +4472,9 @@
       <c r="F96" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H96" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M96" s="3" t="s">
         <v>188</v>
       </c>
@@ -4372,6 +4498,9 @@
       <c r="F97" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H97" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M97" s="3" t="s">
         <v>188</v>
       </c>
@@ -4395,6 +4524,9 @@
       <c r="F98" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H98" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M98" s="3" t="s">
         <v>188</v>
       </c>
@@ -4418,6 +4550,9 @@
       <c r="F99" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H99" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M99" s="3" t="s">
         <v>188</v>
       </c>
@@ -4441,6 +4576,9 @@
       <c r="F100" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H100" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M100" s="3" t="s">
         <v>188</v>
       </c>
@@ -4464,6 +4602,9 @@
       <c r="F101" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H101" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M101" s="3" t="s">
         <v>188</v>
       </c>
@@ -4487,6 +4628,9 @@
       <c r="F102" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H102" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M102" s="3" t="s">
         <v>188</v>
       </c>
@@ -4510,6 +4654,9 @@
       <c r="F103" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H103" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M103" s="3" t="s">
         <v>188</v>
       </c>
@@ -4533,6 +4680,9 @@
       <c r="F104" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H104" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M104" s="3" t="s">
         <v>188</v>
       </c>
@@ -4556,6 +4706,9 @@
       <c r="F105" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H105" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M105" s="3" t="s">
         <v>188</v>
       </c>
@@ -4579,6 +4732,9 @@
       <c r="F106" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H106" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M106" s="3" t="s">
         <v>188</v>
       </c>
@@ -4602,6 +4758,9 @@
       <c r="F107" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H107" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M107" s="3" t="s">
         <v>188</v>
       </c>
@@ -4625,6 +4784,9 @@
       <c r="F108" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H108" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M108" s="3" t="s">
         <v>188</v>
       </c>
@@ -4648,6 +4810,9 @@
       <c r="F109" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H109" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M109" s="3" t="s">
         <v>188</v>
       </c>
@@ -4671,6 +4836,9 @@
       <c r="F110" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H110" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M110" s="3" t="s">
         <v>188</v>
       </c>
@@ -4691,6 +4859,9 @@
       <c r="F111" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H111" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M111" s="3" t="s">
         <v>188</v>
       </c>
@@ -4711,6 +4882,9 @@
       <c r="F112" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H112" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M112" s="3" t="s">
         <v>188</v>
       </c>
@@ -4731,6 +4905,9 @@
       <c r="F113" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H113" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M113" s="3" t="s">
         <v>188</v>
       </c>
@@ -4751,6 +4928,9 @@
       <c r="F114" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H114" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M114" s="3" t="s">
         <v>188</v>
       </c>
@@ -4771,6 +4951,9 @@
       <c r="F115" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H115" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M115" s="3" t="s">
         <v>188</v>
       </c>
@@ -4791,6 +4974,9 @@
       <c r="F116" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H116" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="M116" s="3" t="s">
         <v>188</v>
       </c>
@@ -4811,6 +4997,9 @@
       <c r="F117" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H117" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O117" t="s">
         <v>244</v>
       </c>
@@ -4828,6 +5017,9 @@
       <c r="F118" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H118" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O118" t="s">
         <v>245</v>
       </c>
@@ -4845,6 +5037,9 @@
       <c r="F119" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H119" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O119" t="s">
         <v>246</v>
       </c>
@@ -4862,6 +5057,9 @@
       <c r="F120" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H120" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O120" t="s">
         <v>247</v>
       </c>
@@ -4879,6 +5077,9 @@
       <c r="F121" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H121" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O121" t="s">
         <v>248</v>
       </c>
@@ -4896,6 +5097,9 @@
       <c r="F122" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H122" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O122" t="s">
         <v>249</v>
       </c>
@@ -5446,6 +5650,9 @@
       <c r="G145" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H145" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I145" s="3" t="s">
         <v>187</v>
       </c>
@@ -5569,6 +5776,9 @@
       <c r="G148" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H148" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I148" s="3" t="s">
         <v>187</v>
       </c>
@@ -5601,6 +5811,9 @@
       <c r="F149" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H149" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I149" s="3" t="s">
         <v>187</v>
       </c>
@@ -5636,6 +5849,9 @@
       <c r="F150" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H150" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I150" s="3" t="s">
         <v>187</v>
       </c>
@@ -5665,6 +5881,9 @@
       <c r="F151" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H151" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I151" s="3" t="s">
         <v>187</v>
       </c>
@@ -5700,6 +5919,9 @@
       <c r="F152" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H152" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I152" s="3" t="s">
         <v>187</v>
       </c>
@@ -5735,6 +5957,9 @@
       <c r="F153" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H153" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I153" s="3" t="s">
         <v>187</v>
       </c>
@@ -5750,7 +5975,7 @@
     </row>
     <row r="154" spans="1:15">
       <c r="A154" t="s">
-        <v>26</v>
+        <v>338</v>
       </c>
       <c r="C154" t="s">
         <v>100</v>
@@ -5758,34 +5983,16 @@
       <c r="D154" t="s">
         <v>53</v>
       </c>
-      <c r="E154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L154" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="N154" s="3" t="s">
+      <c r="H154" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O154" t="s">
-        <v>137</v>
+        <v>340</v>
       </c>
     </row>
     <row r="155" spans="1:15">
       <c r="A155" t="s">
-        <v>129</v>
+        <v>339</v>
       </c>
       <c r="C155" t="s">
         <v>52</v>
@@ -5793,28 +6000,16 @@
       <c r="D155" t="s">
         <v>53</v>
       </c>
-      <c r="E155" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I155" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J155" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="N155" s="3" t="s">
+      <c r="H155" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O155" t="s">
-        <v>134</v>
+        <v>341</v>
       </c>
     </row>
     <row r="156" spans="1:15">
       <c r="A156" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C156" t="s">
         <v>100</v>
@@ -5828,6 +6023,9 @@
       <c r="F156" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H156" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I156" s="3" t="s">
         <v>187</v>
       </c>
@@ -5844,15 +6042,15 @@
         <v>187</v>
       </c>
       <c r="O156" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="157" spans="1:15">
       <c r="A157" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="C157" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D157" t="s">
         <v>53</v>
@@ -5863,31 +6061,28 @@
       <c r="F157" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H157" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I157" s="3" t="s">
         <v>187</v>
       </c>
       <c r="J157" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K157" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L157" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="N157" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O157" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="158" spans="1:15">
       <c r="A158" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="C158" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="D158" t="s">
         <v>53</v>
@@ -5898,25 +6093,34 @@
       <c r="F158" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="H158" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="I158" s="3" t="s">
         <v>187</v>
       </c>
       <c r="J158" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="K158" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L158" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="N158" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O158" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="159" spans="1:15">
       <c r="A159" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C159" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="D159" t="s">
         <v>53</v>
@@ -5927,9 +6131,6 @@
       <c r="F159" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G159" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="H159" s="3" t="s">
         <v>187</v>
       </c>
@@ -5945,22 +6146,19 @@
       <c r="L159" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="M159" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="N159" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O159" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
     </row>
     <row r="160" spans="1:15">
       <c r="A160" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="C160" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D160" t="s">
         <v>53</v>
@@ -5971,9 +6169,6 @@
       <c r="F160" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G160" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="H160" s="3" t="s">
         <v>187</v>
       </c>
@@ -5983,25 +6178,19 @@
       <c r="J160" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K160" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L160" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="N160" s="3" t="s">
         <v>187</v>
       </c>
       <c r="O160" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
     </row>
     <row r="161" spans="1:15">
       <c r="A161" t="s">
-        <v>236</v>
+        <v>29</v>
       </c>
       <c r="C161" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D161" t="s">
         <v>53</v>
@@ -6010,39 +6199,39 @@
         <v>187</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M161" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N161" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="O161" s="4" t="s">
-        <v>237</v>
+        <v>187</v>
+      </c>
+      <c r="O161" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="162" spans="1:15">
       <c r="A162" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C162" t="s">
         <v>101</v>
@@ -6056,25 +6245,37 @@
       <c r="F162" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="G162" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="H162" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="I162" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J162" s="3" t="s">
         <v>187</v>
       </c>
       <c r="K162" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="L162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N162" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="O162" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="163" spans="1:15">
       <c r="A163" t="s">
-        <v>32</v>
+        <v>236</v>
       </c>
       <c r="C163" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D163" t="s">
         <v>53</v>
@@ -6083,71 +6284,144 @@
         <v>187</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L163" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="M163" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="N163" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O163" t="s">
-        <v>37</v>
+        <v>188</v>
+      </c>
+      <c r="O163" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="164" spans="1:15">
       <c r="A164" t="s">
+        <v>31</v>
+      </c>
+      <c r="C164" t="s">
+        <v>101</v>
+      </c>
+      <c r="D164" t="s">
+        <v>53</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O164" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15">
+      <c r="A165" t="s">
+        <v>32</v>
+      </c>
+      <c r="C165" t="s">
+        <v>36</v>
+      </c>
+      <c r="D165" t="s">
+        <v>53</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N165" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O165" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
+      <c r="A166" t="s">
         <v>33</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C166" t="s">
         <v>35</v>
       </c>
-      <c r="D164" t="s">
-        <v>53</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="N164" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O164" t="s">
+      <c r="D166" t="s">
+        <v>53</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N166" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O166" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>